<commit_message>
HCW NS text added
</commit_message>
<xml_diff>
--- a/abstracts/abstracts_amended.xlsx
+++ b/abstracts/abstracts_amended.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phil\Documents\yearbook2019\abstracts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heatherw\Documents\yearbook201920\abstracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB38421-42DA-473D-8196-56724BDF5CBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3B0593-8896-4DBD-9F7C-B83AAD1847DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8955" yWindow="-13950" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="abstracts_amended" sheetId="1" r:id="rId1"/>
@@ -2871,8 +2871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="F80" workbookViewId="0">
+      <selection activeCell="K88" sqref="K88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6436,10 +6436,10 @@
         <v>19</v>
       </c>
       <c r="J87" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="K87" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="L87" t="s">
         <v>22</v>

</xml_diff>